<commit_message>
Überarbeitung Grafiken und Texte
</commit_message>
<xml_diff>
--- a/01_Bundestagswahl_2025/data/Wahl-O-Mat Bundestagswahl 2025_Datensatz_v1.01.xlsx
+++ b/01_Bundestagswahl_2025/data/Wahl-O-Mat Bundestagswahl 2025_Datensatz_v1.01.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markheckmann/Workspace/tmp/wahlomat/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markheckmann/Workspace/tmp/wahlomat/01_Bundestagswahl_2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4553096C-2C4F-F842-97B0-8ACEA28A7C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE170C8-7948-424D-B79E-7A5AF48B0DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="17260" activeTab="2" xr2:uid="{4CB89484-2765-4C9E-98CC-EB836685529E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="17260" activeTab="3" xr2:uid="{4CB89484-2765-4C9E-98CC-EB836685529E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hinweis zur Verwendung" sheetId="2" r:id="rId1"/>
     <sheet name="Änderungen" sheetId="3" r:id="rId2"/>
     <sheet name="Datensatz BTW 2025" sheetId="1" r:id="rId3"/>
+    <sheet name="Kurzform" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Änderungen!$A$3:$G$3</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6283" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6401" uniqueCount="1089">
   <si>
     <t>SPD</t>
   </si>
@@ -3180,6 +3181,123 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>These: Kurzform</t>
+  </si>
+  <si>
+    <t>Militärhilfe für Ukraine fortsetzen</t>
+  </si>
+  <si>
+    <t>Erneuerbare Energien finanziell fördern</t>
+  </si>
+  <si>
+    <t>Tempolimit auf Autobahnen einführen</t>
+  </si>
+  <si>
+    <t>Mietpreisbegrenzung beibehalten</t>
+  </si>
+  <si>
+    <t>Gesichtserkennung an Bahnhöfen erlauben</t>
+  </si>
+  <si>
+    <t>Stromkosten-Ausgleich für Unternehmen</t>
+  </si>
+  <si>
+    <t>Rentenabschläge nach 40 Jahren abschaffen</t>
+  </si>
+  <si>
+    <t>Fachkräfteanwerbung aus Ausland fördern</t>
+  </si>
+  <si>
+    <t>Kernenergie zur Stromerzeugung nutzen</t>
+  </si>
+  <si>
+    <t>Spitzensteuersatz anheben</t>
+  </si>
+  <si>
+    <t>Schulpolitik-Befugnisse für Bund stärken</t>
+  </si>
+  <si>
+    <t>Rüstungsexporte nach Israel erlauben</t>
+  </si>
+  <si>
+    <t>Frauenquote in Vorständen abschaffen</t>
+  </si>
+  <si>
+    <t>Ökologische Landwirtschaft stärker fördern</t>
+  </si>
+  <si>
+    <t>Rechtsextremismus-Projekte verstärkt fördern</t>
+  </si>
+  <si>
+    <t>BAföG einkommensabhängig belassen</t>
+  </si>
+  <si>
+    <t>Schuldenbremse im Grundgesetz beibehalten</t>
+  </si>
+  <si>
+    <t>Arbeitserlaubnis für Asylsuchende sofort</t>
+  </si>
+  <si>
+    <t>Klimaneutralitätsziel aufgeben</t>
+  </si>
+  <si>
+    <t>35-Stunden-Woche gesetzlich einführen</t>
+  </si>
+  <si>
+    <t>Euro durch nationale Währung ersetzen</t>
+  </si>
+  <si>
+    <t>Schienenverkehr vor Straßenverkehr priorisieren</t>
+  </si>
+  <si>
+    <t>Ehrenamtliche Tätigkeiten für Rente anrechnen</t>
+  </si>
+  <si>
+    <t>Grundsteuer auf Mieter umlegen</t>
+  </si>
+  <si>
+    <t>Streikrecht in kritischen Bereichen einschränken</t>
+  </si>
+  <si>
+    <t>Volksentscheide auf Bundesebene ermöglichen</t>
+  </si>
+  <si>
+    <t>Strafbarkeit ab 14 einführen</t>
+  </si>
+  <si>
+    <t>EU-Zölle auf E-Autos abschaffen</t>
+  </si>
+  <si>
+    <t>Doppelstaatsbürgerschaft weiterhin ermöglichen</t>
+  </si>
+  <si>
+    <t>Soziales Pflichtjahr für Jugendliche einführen</t>
+  </si>
+  <si>
+    <t>Fossile Heizungen weiterhin erlauben</t>
+  </si>
+  <si>
+    <t>Mindestlohn auf 15 Euro erhöhen</t>
+  </si>
+  <si>
+    <t>Beratungspflicht vor Schwangerschaftsabbruch</t>
+  </si>
+  <si>
+    <t>Menschenrechtskontrolle durch Unternehmen</t>
+  </si>
+  <si>
+    <t>Gesetzliche Krankenversicherungspflicht für alle</t>
+  </si>
+  <si>
+    <t>„Verantwortung vor Gott“ im GG beibehalten</t>
+  </si>
+  <si>
+    <t>aus EU-Staat eingereiste Asylsuchende abweisen</t>
+  </si>
+  <si>
+    <t>Bürgergeld bei Ablehnung Stellenangebot streichen</t>
   </si>
 </sst>
 </file>
@@ -3736,8 +3854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC3ABC7-14C4-4B1F-AA13-23DBE8944207}">
   <dimension ref="A1:H1065"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A670" workbookViewId="0">
+      <selection activeCell="D670" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31051,4 +31169,570 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3005A4-E98D-6042-8316-7FE7564D74A4}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="105.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>